<commit_message>
added qrc images and hard coded paths to work with one file exe
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Hassan</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Ahmed2</t>
+  </si>
+  <si>
+    <t>variable</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:AA618"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -474,6 +477,9 @@
       </c>
       <c r="B2" s="7">
         <v>1120641378</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>